<commit_message>
09_study(For Each Row in Data Table, Anchor Base, Find Element)
</commit_message>
<xml_diff>
--- a/과제_20230926/Rsult.xlsx
+++ b/과제_20230926/Rsult.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\GitHub\과제_20230926\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\git\과제_20230926\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20175" windowHeight="9480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9426" windowHeight="8166"/>
   </bookViews>
   <sheets>
-    <sheet name="지상파" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="케이블" sheetId="4" r:id="rId1"/>
+    <sheet name="종합편성" sheetId="3" r:id="rId2"/>
+    <sheet name="지상파" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,27 +27,184 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>순위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>채널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>프로그램명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>채널</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>시청률</t>
-  </si>
-  <si>
-    <t>숫자시청률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효심이네 각자도생</t>
+  </si>
+  <si>
+    <t>KBS2</t>
+  </si>
+  <si>
+    <t>우당탕탕 패밀리</t>
+  </si>
+  <si>
+    <t>KBS1</t>
+  </si>
+  <si>
+    <t>7인의 탈출</t>
+  </si>
+  <si>
+    <t>SBS</t>
+  </si>
+  <si>
+    <t>7인의 탈출 (재방송)</t>
+  </si>
+  <si>
+    <t>하늘의 인연 (재방송)</t>
+  </si>
+  <si>
+    <t>MBC</t>
+  </si>
+  <si>
+    <t>순정복서</t>
+  </si>
+  <si>
+    <t>순정복서 (재방송)</t>
+  </si>
+  <si>
+    <t>국민사형투표 (재방송)</t>
+  </si>
+  <si>
+    <t>KBS 네트워크 특선 (재방송)</t>
+  </si>
+  <si>
+    <t>프로그램명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시청률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>힙하게</t>
+  </si>
+  <si>
+    <t>JTBC</t>
+  </si>
+  <si>
+    <t>이 연애는 불가항력</t>
+  </si>
+  <si>
+    <t>힙하게 (재방송)</t>
+  </si>
+  <si>
+    <t>이 연애는 불가항력 (재방송)</t>
+  </si>
+  <si>
+    <t>이 연애는 불가항력 (스페셜)</t>
+  </si>
+  <si>
+    <t>순위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로그램명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잔혹한 인턴</t>
+  </si>
+  <si>
+    <t>tvN</t>
+  </si>
+  <si>
+    <t>유괴의 날</t>
+  </si>
+  <si>
+    <t>ENA</t>
+  </si>
+  <si>
+    <t>반짝이는 워터멜론</t>
+  </si>
+  <si>
+    <t>아라문의 검 : 너의 사명을 알리라</t>
+  </si>
+  <si>
+    <t>잔혹한 인턴 (재방송)</t>
+  </si>
+  <si>
+    <t>반짝이는 워터멜론 (재방송)</t>
+  </si>
+  <si>
+    <t>효심이네 각자도생 (재방송)</t>
+  </si>
+  <si>
+    <t>KBS Drama</t>
+  </si>
+  <si>
+    <t>사랑의 불시착 (재방송)</t>
+  </si>
+  <si>
+    <t>tvN STORY</t>
+  </si>
+  <si>
+    <t>JTBC2</t>
+  </si>
+  <si>
+    <t>며느라기 (재방송)</t>
+  </si>
+  <si>
+    <t>MBC 드라마넷</t>
+  </si>
+  <si>
+    <t>며느라기2…ing (재방송)</t>
+  </si>
+  <si>
+    <t>유괴의 날 (재방송)</t>
+  </si>
+  <si>
+    <t>아라문의 검 (재방송)</t>
+  </si>
+  <si>
+    <t>도깨비 (재방송)</t>
+  </si>
+  <si>
+    <t>tvN DRAMA</t>
+  </si>
+  <si>
+    <t>재벌집 막내아들 (재방송)</t>
+  </si>
+  <si>
+    <t>스토브리그 (재방송)</t>
+  </si>
+  <si>
+    <t>SBS Plus</t>
+  </si>
+  <si>
+    <t>같이 살래요 (재방송)</t>
+  </si>
+  <si>
+    <t>EDGETV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,9 +311,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -187,9 +346,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -369,27 +528,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.7"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -400,11 +836,263 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.7"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.7"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.7">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.7"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>